<commit_message>
Changed the Log file name format, Updated Tests
</commit_message>
<xml_diff>
--- a/WebServiceTests/Resources/TestCaseData.xlsx
+++ b/WebServiceTests/Resources/TestCaseData.xlsx
@@ -4,27 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="WebServicexTests" sheetId="2" r:id="rId1"/>
     <sheet name="PostmanTests" sheetId="5" r:id="rId2"/>
     <sheet name="MontanaTests" sheetId="6" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
-    <sheet name="DataValidationWithURI" sheetId="8" r:id="rId5"/>
-    <sheet name="DataValidationWithoutURI" sheetId="10" r:id="rId6"/>
-    <sheet name="NavigationWithURI" sheetId="9" r:id="rId7"/>
-    <sheet name="NavigationWithoutURI" sheetId="11" r:id="rId8"/>
-    <sheet name="NavigationWithoutHeaders" sheetId="14" r:id="rId9"/>
+    <sheet name="DataValidationTestsWithURI" sheetId="8" r:id="rId5"/>
+    <sheet name="DataValidationTestsWithoutURI" sheetId="10" r:id="rId6"/>
+    <sheet name="NavigationTestsWithURI" sheetId="9" r:id="rId7"/>
+    <sheet name="NavigationTestsWithoutURI" sheetId="11" r:id="rId8"/>
+    <sheet name="NavigationTestsWithoutHeaders" sheetId="14" r:id="rId9"/>
     <sheet name="Others" sheetId="12" r:id="rId10"/>
-    <sheet name="Calculator" sheetId="13" r:id="rId11"/>
+    <sheet name="CalculatorTestsWithURI" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="140">
   <si>
     <t>Method</t>
   </si>
@@ -545,9 +545,6 @@
 &lt;/soap:Envelope&gt;</t>
   </si>
   <si>
-    <t>PeriodicTable\AtomicNumber.xml</t>
-  </si>
-  <si>
     <t>http://apilayer.net/api/check?access_key=0af0be9cbdd897e592a3008443a29a55&amp;email=webserviceapi@outlook.com&amp;smtp=1&amp;format=1</t>
   </si>
   <si>
@@ -688,9 +685,6 @@
     <t>TC_getNearByCityName</t>
   </si>
   <si>
-    <t>navigation\ResponseGetNearByCityName.txt</t>
-  </si>
-  <si>
     <t>/api/check?access_key=0af0be9cbdd897e592a3008443a29a55&amp;email=webserviceapi@outlook.com&amp;smtp=1&amp;format=1</t>
   </si>
   <si>
@@ -736,9 +730,6 @@
     &lt;/GetCitiesByCountry&gt;
   &lt;/soap:Body&gt;
 &lt;/soap:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>"&lt;?xml version=\"1.0\" encoding=\"utf-8\"?&gt;&lt;soap:Envelope xmlns:soap=\"http://schemas.xmlsoap.org/soap/envelope/\" xmlns:xsi=\"http://www.w3.org/2001/XMLSchema-instance\" xmlns:xsd=\"http://www.w3.org/2001/XMLSchema\"&gt;&lt;soap:Body&gt;&lt;GetCitiesByCountryResponse xmlns=\"http://www.webserviceX.NET\"&gt;&lt;GetCitiesByCountryResult&gt;&amp;lt;NewDataSet&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;British Indian Ocean Territory&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Diego Garcia&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Ahmadabad&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Akola&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Aurangabad Chikalthan Aerodrome&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bombay / Santacruz&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bilaspur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bhuj-Rudramata&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Belgaum / Sambra&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bhopal / Bairagarh&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bhaunagar&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Goa / Dabolim Airport&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Indore&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Jabalpur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Khandwa&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Kolhapur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Nagpur Sonegaon&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Rajkot&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Sholapur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Agartala&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Siliguri&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bhubaneswar&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Calcutta / Dum Dum&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Car Nicobar&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Gorakhpur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Gauhati&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Gaya&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Imphal Tulihal&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Jharsuguda&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Jamshedpur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;North Lakhimpur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Dibrugarh / Mohanbari&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Port Blair&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Patna&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;M. O. Ranchi&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Agra&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Allahabad / Bamhrauli&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Amritsar&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Varanasi / Babatpur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bareilly&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Kanpur / Chakeri&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;New Delhi / Safdarjung&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;New Delhi / Palam&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Gwalior&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Hissar&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Jhansi&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Jodhpur&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Jaipur / Sanganer&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Kota Aerodrome&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Lucknow / Amausi&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Satna&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Udaipur Dabok&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Bellary&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Vijayawada / Gannavaram&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Coimbatore / Peelamedu&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Cochin / Willingdon&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Cuddapah&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Hyderabad Airport&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Madurai&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Mangalore / Bajpe&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Madras / Minambakkam&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Tiruchchirapalli&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Thiruvananthapuram&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n  &amp;lt;Table&amp;gt;\r\n    &amp;lt;Country&amp;gt;India&amp;lt;/Country&amp;gt;\r\n    &amp;lt;City&amp;gt;Vellore&amp;lt;/City&amp;gt;\r\n  &amp;lt;/Table&amp;gt;\r\n&amp;lt;/NewDataSet&amp;gt;&lt;/GetCitiesByCountryResult&gt;&lt;/GetCitiesByCountryResponse&gt;&lt;/soap:Body&gt;&lt;/soap:Envelope&gt;"</t>
   </si>
   <si>
     <t>Content-Type:text/xml; charset=utf-8
@@ -759,9 +750,6 @@
     <t>TC_textToBraille</t>
   </si>
   <si>
-    <t>Others\TC_textToBraille.xml</t>
-  </si>
-  <si>
     <t>/braille.asmx</t>
   </si>
   <si>
@@ -773,13 +761,80 @@
   <si>
     <t>Content-Type:text/xml; charset=utf-8
 SOAPAction:"http://tempuri.org/Add"</t>
+  </si>
+  <si>
+    <t>TC_Sub</t>
+  </si>
+  <si>
+    <t>Content-Type: text/xml; charset=utf-8
+SOAPAction: "http://tempuri.org/Subtract"</t>
+  </si>
+  <si>
+    <t>TC_Mul</t>
+  </si>
+  <si>
+    <t>TC_Div</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="utf-8"?&gt;
+&lt;soap:Envelope xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:soap="http://schemas.xmlsoap.org/soap/envelope/"&gt;
+  &lt;soap:Body&gt;
+    &lt;Subtract xmlns="http://tempuri.org/"&gt;
+      &lt;intA&gt;5&lt;/intA&gt;
+      &lt;intB&gt;3&lt;/intB&gt;
+    &lt;/Subtract&gt;
+  &lt;/soap:Body&gt;
+&lt;/soap:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>Content-Type: text/xml; charset=utf-8
+SOAPAction: "http://tempuri.org/Multiply"</t>
+  </si>
+  <si>
+    <t>Content-Type: text/xml; charset=utf-8
+SOAPAction: "http://tempuri.org/Divide"</t>
+  </si>
+  <si>
+    <t>OtherTests\AtomicNumber.xml</t>
+  </si>
+  <si>
+    <t>OtherTests\TC_textToBraille.xml</t>
+  </si>
+  <si>
+    <t>Navigation\ResponseGetNearByCityName.txt</t>
+  </si>
+  <si>
+    <t>Navigation\ResponseGetCitiesByCountry.xml</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="utf-8"?&gt;
+&lt;soap:Envelope xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:soap="http://schemas.xmlsoap.org/soap/envelope/"&gt;
+  &lt;soap:Body&gt;
+    &lt;Divide xmlns="http://tempuri.org/"&gt;
+      &lt;intA&gt;6&lt;/intA&gt;
+      &lt;intB&gt;2&lt;/intB&gt;
+    &lt;/Divide&gt;
+  &lt;/soap:Body&gt;
+&lt;/soap:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>Calculator\ResponsePerformAddition.xml</t>
+  </si>
+  <si>
+    <t>Calculator\ResponsePerformSubtraction.xml</t>
+  </si>
+  <si>
+    <t>Calculator\ResponsePerformMultiplication.xml</t>
+  </si>
+  <si>
+    <t>Calculator\ResponsePerformDivision.xml</t>
   </si>
   <si>
     <t>&lt;?xml version="1.0" encoding="utf-8"?&gt;
 &lt;soap:Envelope xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:soap="http://schemas.xmlsoap.org/soap/envelope/"&gt;
   &lt;soap:Body&gt;
     &lt;Add xmlns="http://tempuri.org/"&gt;
-      &lt;intA&gt;2&lt;/intA&gt;
+      &lt;intA&gt;5&lt;/intA&gt;
       &lt;intB&gt;3&lt;/intB&gt;
     &lt;/Add&gt;
   &lt;/soap:Body&gt;
@@ -787,12 +842,13 @@
   </si>
   <si>
     <t>&lt;?xml version="1.0" encoding="utf-8"?&gt;
-&lt;soap:Envelope xmlns:soap="http://schemas.xmlsoap.org/soap/envelope/" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema"&gt;
-    &lt;soap:Body&gt;
-        &lt;AddResponse xmlns="http://tempuri.org/"&gt;
-            &lt;AddResult&gt;5&lt;/AddResult&gt;
-        &lt;/AddResponse&gt;
-    &lt;/soap:Body&gt;
+&lt;soap:Envelope xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:soap="http://schemas.xmlsoap.org/soap/envelope/"&gt;
+  &lt;soap:Body&gt;
+    &lt;Multiply xmlns="http://tempuri.org/"&gt;
+      &lt;intA&gt;3&lt;/intA&gt;
+      &lt;intB&gt;5&lt;/intB&gt;
+    &lt;/Multiply&gt;
+  &lt;/soap:Body&gt;
 &lt;/soap:Envelope&gt;</t>
   </si>
 </sst>
@@ -859,7 +915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -870,6 +926,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1145,8 +1204,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F3" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F5"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
@@ -1593,7 +1652,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1937,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1918,7 +1977,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,22 +2009,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1989,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,40 +2082,96 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>124</v>
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2470,7 +2585,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,10 +2620,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -2516,15 +2631,15 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -2532,15 +2647,15 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -2548,15 +2663,15 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -2564,67 +2679,67 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2653,11 +2768,12 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="69.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2683,10 +2799,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -2694,15 +2810,15 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -2710,15 +2826,15 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -2726,15 +2842,15 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -2742,67 +2858,67 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2828,12 +2944,12 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="59.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="43.140625" customWidth="1"/>
@@ -2862,25 +2978,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -2888,27 +3004,27 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>115</v>
+      <c r="D4" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2928,8 +3044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,25 +3076,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -2986,27 +3102,27 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3027,7 +3143,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3059,22 +3175,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CalculatorTests, Included OthersTest, AtomicNumber.xml
</commit_message>
<xml_diff>
--- a/WebServiceTests/Resources/TestCaseData.xlsx
+++ b/WebServiceTests/Resources/TestCaseData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="WebServicexTests" sheetId="2" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="NavigationTestsWithoutHeaders" sheetId="14" r:id="rId9"/>
     <sheet name="Others" sheetId="12" r:id="rId10"/>
     <sheet name="CalculatorTestsWithURI" sheetId="13" r:id="rId11"/>
+    <sheet name="CalculatorTestsWithoutURI" sheetId="15" r:id="rId12"/>
+    <sheet name="CalculatorTestsWithoutHeaders" sheetId="16" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="141">
   <si>
     <t>Method</t>
   </si>
@@ -673,9 +675,6 @@
     <t>{"success":true,"results":[{"language_code":"fr","language_name":"French","probability":20.112935852276,"percentage":100,"reliable_result":true}]}</t>
   </si>
   <si>
-    <t>http://api.geonames.org/postalCodeSearchJSON?postalcode=607802&amp;maxRows=19&amp;username=webserviceapi</t>
-  </si>
-  <si>
     <t>Navigation\ResponseGetCitiesByPostalCode.txt</t>
   </si>
   <si>
@@ -704,9 +703,6 @@
   </si>
   <si>
     <t>/api/validate?access_key=61054062e54a845e89e158ded3ee383c&amp;number=+14158586273&amp;country_code=&amp;format=1</t>
-  </si>
-  <si>
-    <t>/postalCodeSearchJSON?postalcode=607802&amp;maxRows=19&amp;username=webserviceapi</t>
   </si>
   <si>
     <t>/findNearbyPlaceNameJSON?lat=12.95&amp;lng=80.14&amp;username=webserviceapi</t>
@@ -850,6 +846,15 @@
     &lt;/Multiply&gt;
   &lt;/soap:Body&gt;
 &lt;/soap:Envelope&gt;</t>
+  </si>
+  <si>
+    <t>/calculator.asmx</t>
+  </si>
+  <si>
+    <t>http://api.geonames.org/postalCodeSearchJSON?postalcode=600077&amp;maxRows=19&amp;username=webserviceapi</t>
+  </si>
+  <si>
+    <t>/postalCodeSearchJSON?postalcode=600077&amp;maxRows=19&amp;username=webserviceapi</t>
   </si>
 </sst>
 </file>
@@ -934,7 +939,55 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="96">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1186,11 +1239,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:F9"/>
   <sortState ref="A2:F12">
     <sortCondition ref="B1"/>
   </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="93"/>
+    <tableColumn id="2" name="URISegment" dataDxfId="92"/>
+    <tableColumn id="3" name="Method" dataDxfId="91"/>
+    <tableColumn id="4" name="Headers" dataDxfId="90"/>
+    <tableColumn id="5" name="PostBody" dataDxfId="89"/>
+    <tableColumn id="6" name="Expected Response Body" dataDxfId="88"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:F5"/>
+  <sortState ref="A2:F14">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="21"/>
+    <tableColumn id="2" name="URISegment" dataDxfId="20"/>
+    <tableColumn id="3" name="Method" dataDxfId="19"/>
+    <tableColumn id="4" name="Headers" dataDxfId="18"/>
+    <tableColumn id="5" name="PostBody" dataDxfId="17"/>
+    <tableColumn id="6" name="Expected Response Body" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table156891012" displayName="Table156891012" ref="A1:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F5"/>
+  <sortState ref="A2:F14">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="13"/>
+    <tableColumn id="2" name="URISegment" dataDxfId="12"/>
+    <tableColumn id="3" name="Method" dataDxfId="11"/>
+    <tableColumn id="4" name="Headers" dataDxfId="10"/>
+    <tableColumn id="5" name="PostBody" dataDxfId="9"/>
+    <tableColumn id="6" name="Expected Response Body" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table156891013" displayName="Table156891013" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F5"/>
+  <sortState ref="A2:F14">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" name="URISegment" dataDxfId="4"/>
+    <tableColumn id="3" name="Method" dataDxfId="2"/>
+    <tableColumn id="4" name="Headers" dataDxfId="0"/>
+    <tableColumn id="5" name="PostBody" dataDxfId="1"/>
+    <tableColumn id="6" name="Expected Response Body" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F15" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+  <autoFilter ref="A1:F15"/>
+  <sortState ref="A2:F14">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="85"/>
+    <tableColumn id="2" name="URISegment" dataDxfId="84"/>
+    <tableColumn id="3" name="Method" dataDxfId="83"/>
+    <tableColumn id="4" name="Headers" dataDxfId="82"/>
+    <tableColumn id="5" name="PostBody" dataDxfId="81"/>
+    <tableColumn id="6" name="Expected Response Body" dataDxfId="80"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F5" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+  <autoFilter ref="A1:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="77"/>
     <tableColumn id="2" name="URISegment" dataDxfId="76"/>
@@ -1203,27 +1343,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F5"/>
-  <sortState ref="A2:F14">
-    <sortCondition ref="B1"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" name="URISegment" dataDxfId="4"/>
-    <tableColumn id="3" name="Method" dataDxfId="3"/>
-    <tableColumn id="4" name="Headers" dataDxfId="2"/>
-    <tableColumn id="5" name="PostBody" dataDxfId="1"/>
-    <tableColumn id="6" name="Expected Response Body" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F15" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="A1:F15"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:F9" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="A1:F9"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
@@ -1239,9 +1361,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
-  <autoFilter ref="A1:F5"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table157" displayName="Table157" ref="A1:F9" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <autoFilter ref="A1:F9"/>
+  <sortState ref="A2:F14">
+    <sortCondition ref="B1"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="61"/>
     <tableColumn id="2" name="URISegment" dataDxfId="60"/>
@@ -1254,9 +1379,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:F9" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <autoFilter ref="A1:F9"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:F4" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A1:F4"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
@@ -1272,9 +1397,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table157" displayName="Table157" ref="A1:F9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A1:F9"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1568" displayName="Table1568" ref="A1:F4" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="A1:F4"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
@@ -1290,15 +1415,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:F4" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A1:F4"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table15611" displayName="Table15611" ref="A1:F2" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A1:F2"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="37"/>
-    <tableColumn id="2" name="URISegment" dataDxfId="36"/>
+    <tableColumn id="2" name="URISegment" dataDxfId="36" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" name="Method" dataDxfId="35"/>
     <tableColumn id="4" name="Headers" dataDxfId="34"/>
     <tableColumn id="5" name="PostBody" dataDxfId="33"/>
@@ -1308,9 +1433,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1568" displayName="Table1568" ref="A1:F4" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:F4"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table15689" displayName="Table15689" ref="A1:F3" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:F3"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
@@ -1321,42 +1446,6 @@
     <tableColumn id="4" name="Headers" dataDxfId="26"/>
     <tableColumn id="5" name="PostBody" dataDxfId="25"/>
     <tableColumn id="6" name="Expected Response Body" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table15611" displayName="Table15611" ref="A1:F2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:F2"/>
-  <sortState ref="A2:F14">
-    <sortCondition ref="B1"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="21"/>
-    <tableColumn id="2" name="URISegment" dataDxfId="20" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Method" dataDxfId="19"/>
-    <tableColumn id="4" name="Headers" dataDxfId="18"/>
-    <tableColumn id="5" name="PostBody" dataDxfId="17"/>
-    <tableColumn id="6" name="Expected Response Body" dataDxfId="16"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table15689" displayName="Table15689" ref="A1:F3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F3"/>
-  <sortState ref="A2:F14">
-    <sortCondition ref="B1"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="13"/>
-    <tableColumn id="2" name="URISegment" dataDxfId="12"/>
-    <tableColumn id="3" name="Method" dataDxfId="11"/>
-    <tableColumn id="4" name="Headers" dataDxfId="10"/>
-    <tableColumn id="5" name="PostBody" dataDxfId="9"/>
-    <tableColumn id="6" name="Expected Response Body" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1937,7 +2026,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2009,22 +2098,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2050,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,82 +2172,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2172,6 +2261,254 @@
   <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
     <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
+    <col min="6" max="6" width="55.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://www.dneonline.com/calculator.asmx"/>
+    <hyperlink ref="B3:B5" r:id="rId2" display="http://www.dneonline.com/calculator.asmx"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2802,7 +3139,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -2818,7 +3155,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -2834,7 +3171,7 @@
         <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -2850,7 +3187,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -2866,7 +3203,7 @@
         <v>83</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -2881,7 +3218,7 @@
         <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -2896,7 +3233,7 @@
         <v>86</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -2911,7 +3248,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -2944,7 +3281,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,22 +3318,22 @@
         <v>90</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -3004,27 +3341,27 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3045,7 +3382,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,22 +3416,22 @@
         <v>90</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -3102,12 +3439,12 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>66</v>
@@ -3116,13 +3453,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3143,7 +3480,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,20 +3514,20 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DataValidationTestsException class file
</commit_message>
<xml_diff>
--- a/WebServiceTests/Resources/TestCaseData.xlsx
+++ b/WebServiceTests/Resources/TestCaseData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WebServicexTests" sheetId="2" r:id="rId1"/>
@@ -1301,10 +1301,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="5"/>
     <tableColumn id="2" name="URISegment" dataDxfId="4"/>
-    <tableColumn id="3" name="Method" dataDxfId="2"/>
-    <tableColumn id="4" name="Headers" dataDxfId="0"/>
+    <tableColumn id="3" name="Method" dataDxfId="3"/>
+    <tableColumn id="4" name="Headers" dataDxfId="2"/>
     <tableColumn id="5" name="PostBody" dataDxfId="1"/>
-    <tableColumn id="6" name="Expected Response Body" dataDxfId="3"/>
+    <tableColumn id="6" name="Expected Response Body" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2396,7 +2396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
@@ -2922,13 +2922,13 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="118.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="44.140625" customWidth="1"/>
@@ -3280,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3348,7 +3348,7 @@
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -3382,11 +3382,12 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="66.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Changed SerializeXML, Added XmlSerialize tests
</commit_message>
<xml_diff>
--- a/WebServiceTests/Resources/TestCaseData.xlsx
+++ b/WebServiceTests/Resources/TestCaseData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="WebServicexTests" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="142">
   <si>
     <t>Method</t>
   </si>
@@ -855,6 +855,9 @@
   </si>
   <si>
     <t>/postalCodeSearchJSON?postalcode=600077&amp;maxRows=19&amp;username=webserviceapi</t>
+  </si>
+  <si>
+    <t>TC_Add_Object</t>
   </si>
 </sst>
 </file>
@@ -1257,8 +1260,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F6" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:F6"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
@@ -2137,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,17 +2253,36 @@
         <v>135</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3280,7 +3302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Serialized tests in CalculatorTests
</commit_message>
<xml_diff>
--- a/WebServiceTests/Resources/TestCaseData.xlsx
+++ b/WebServiceTests/Resources/TestCaseData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="145">
   <si>
     <t>Method</t>
   </si>
@@ -858,6 +858,15 @@
   </si>
   <si>
     <t>TC_Add_Object</t>
+  </si>
+  <si>
+    <t>TC_Sub_Object</t>
+  </si>
+  <si>
+    <t>TC_Mul_Object</t>
+  </si>
+  <si>
+    <t>TC_Div_Object</t>
   </si>
 </sst>
 </file>
@@ -1260,8 +1269,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F6" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1568910" displayName="Table1568910" ref="A1:F9" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:F9"/>
   <sortState ref="A2:F14">
     <sortCondition ref="B1"/>
   </sortState>
@@ -2140,10 +2149,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,6 +2280,60 @@
         <v>132</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -2278,11 +2341,14 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changes in Logger, CreateResource Serialization and DeSerialization, Added JSONFormatter in Utils
</commit_message>
<xml_diff>
--- a/WebServiceTests/Resources/TestCaseData.xlsx
+++ b/WebServiceTests/Resources/TestCaseData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="13395" windowHeight="7500" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="WebServicexTests" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="151">
   <si>
     <t>Method</t>
   </si>
@@ -870,6 +870,21 @@
   </si>
   <si>
     <t>Below 4 TC's doesn't contains PostBody</t>
+  </si>
+  <si>
+    <t>TC_createResource</t>
+  </si>
+  <si>
+    <t>http://jsonplaceholder.typicode.com/posts</t>
+  </si>
+  <si>
+    <t>Content-Type:application/json</t>
+  </si>
+  <si>
+    <t>OtherTests\TC_createResource.txt</t>
+  </si>
+  <si>
+    <t>{"title": "Create","body": "New Body","userId":1125}</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2078,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,20 +2145,33 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://www.webserviceX.NET//braille.asmx"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>